<commit_message>
updated the vanpool page correctly this time
</commit_message>
<xml_diff>
--- a/rider/monthly/2016_9.xlsx
+++ b/rider/monthly/2016_9.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CTR-External (6040)\CMAQ12-13 (6085)\go\reports\rider\monthly\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Ridership" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Weekday</t>
   </si>
@@ -116,13 +121,34 @@
   </si>
   <si>
     <t>23 Sep 2016</t>
+  </si>
+  <si>
+    <t>24 Sep 2016</t>
+  </si>
+  <si>
+    <t>25 Sep 2016</t>
+  </si>
+  <si>
+    <t>26 Sep 2016</t>
+  </si>
+  <si>
+    <t>27 Sep 2016</t>
+  </si>
+  <si>
+    <t>28 Sep 2016</t>
+  </si>
+  <si>
+    <t>29 Sep 2016</t>
+  </si>
+  <si>
+    <t>30 Sep 2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,12 +185,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -182,12 +226,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -206,9 +252,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$23</c:f>
+              <c:f>Ridership!$B$2:$B$30</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>01 Sep 2016</c:v>
                 </c:pt>
@@ -274,85 +320,128 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>23 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30 Sep 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$C$2:$C$23</c:f>
+              <c:f>Ridership!$C$2:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>199</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>137</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>221</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>74</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>203</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>237</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>209</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>252</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>220</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>217</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>239</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>215</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>180</c:v>
+                  <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>277</c:v>
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>266</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -372,9 +461,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$23</c:f>
+              <c:f>Ridership!$B$2:$B$30</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>01 Sep 2016</c:v>
                 </c:pt>
@@ -440,85 +529,128 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>23 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30 Sep 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$D$2:$D$23</c:f>
+              <c:f>Ridership!$D$2:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>106.27</c:v>
+                  <c:v>105.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.55</c:v>
+                  <c:v>102.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.66</c:v>
+                  <c:v>48.88</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.49</c:v>
+                  <c:v>37.450000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>103.98</c:v>
+                  <c:v>104.09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>109.74</c:v>
+                  <c:v>109.64</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>108.45</c:v>
+                  <c:v>108.23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>104.88</c:v>
+                  <c:v>104.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49.37</c:v>
+                  <c:v>49.59</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.19</c:v>
+                  <c:v>38.130000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>102.15</c:v>
+                  <c:v>101.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>106.4</c:v>
+                  <c:v>106.89</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>111.57</c:v>
+                  <c:v>112.06</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>111.11</c:v>
+                  <c:v>110.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>107.14</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49.58</c:v>
+                  <c:v>49.79</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>38.89</c:v>
+                  <c:v>38.81</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>104.49</c:v>
+                  <c:v>104.35</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>108.77</c:v>
+                  <c:v>108.89</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113.45</c:v>
+                  <c:v>114.05</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>112.36</c:v>
+                  <c:v>111.76</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>110.4</c:v>
+                  <c:v>109.94</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>50.87</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39.33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>106.72</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>110.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>115.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>113.32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>112.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -538,9 +670,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$23</c:f>
+              <c:f>Ridership!$B$2:$B$30</c:f>
               <c:strCache>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>01 Sep 2016</c:v>
                 </c:pt>
@@ -606,18 +738,39 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>23 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29 Sep 2016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30 Sep 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$E$2:$E$23</c:f>
+              <c:f>Ridership!$E$2:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>78.65</c:v>
+                  <c:v>78.650000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>78.81</c:v>
@@ -629,7 +782,7 @@
                   <c:v>79.14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.46</c:v>
+                  <c:v>79.459999999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>79.62</c:v>
@@ -641,13 +794,13 @@
                   <c:v>79.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.1</c:v>
+                  <c:v>80.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>80.27</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80.43</c:v>
+                  <c:v>80.430000000000007</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>80.59</c:v>
@@ -659,13 +812,13 @@
                   <c:v>80.91</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>81.07</c:v>
+                  <c:v>81.069999999999993</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>81.23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>81.4</c:v>
+                  <c:v>81.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>81.56</c:v>
@@ -681,20 +834,51 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>82.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>82.36</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>82.53</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>82.69</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>82.85</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83.01</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>83.17</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>83.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50010001"/>
-        <c:axId val="50010002"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="288816616"/>
+        <c:axId val="288816224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50010001"/>
+        <c:axId val="288816616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -712,20 +896,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010002"/>
+        <c:crossAx val="288816224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50010002"/>
+        <c:axId val="288816224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -744,20 +933,24 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010001"/>
+        <c:crossAx val="288816616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -773,13 +966,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -845,7 +1038,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -877,9 +1070,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -911,6 +1105,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1086,21 +1281,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1125,16 +1316,16 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D2">
-        <v>106.27</v>
+        <v>105.94</v>
       </c>
       <c r="E2">
-        <v>78.65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>78.650000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1142,16 +1333,16 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D3">
-        <v>102.55</v>
+        <v>102.76</v>
       </c>
       <c r="E3">
         <v>78.81</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1162,13 +1353,13 @@
         <v>97</v>
       </c>
       <c r="D4">
-        <v>48.66</v>
+        <v>48.88</v>
       </c>
       <c r="E4">
         <v>78.97</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1176,16 +1367,16 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5">
-        <v>37.49</v>
+        <v>37.450000000000003</v>
       </c>
       <c r="E5">
         <v>79.14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1193,16 +1384,16 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="D6">
-        <v>103.98</v>
+        <v>104.09</v>
       </c>
       <c r="E6">
-        <v>79.46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>79.459999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1210,16 +1401,16 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="D7">
-        <v>109.74</v>
+        <v>109.64</v>
       </c>
       <c r="E7">
         <v>79.62</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1227,16 +1418,16 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D8">
-        <v>108.45</v>
+        <v>108.23</v>
       </c>
       <c r="E8">
         <v>79.78</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1244,16 +1435,16 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D9">
-        <v>104.88</v>
+        <v>104.9</v>
       </c>
       <c r="E9">
         <v>79.94</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1264,13 +1455,13 @@
         <v>85</v>
       </c>
       <c r="D10">
-        <v>49.37</v>
+        <v>49.59</v>
       </c>
       <c r="E10">
-        <v>80.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>80.099999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1278,16 +1469,16 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11">
-        <v>38.19</v>
+        <v>38.130000000000003</v>
       </c>
       <c r="E11">
         <v>80.27</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1295,16 +1486,16 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="D12">
-        <v>102.15</v>
+        <v>101.75</v>
       </c>
       <c r="E12">
-        <v>80.43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>80.430000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1312,16 +1503,16 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <v>237</v>
+        <v>258</v>
       </c>
       <c r="D13">
-        <v>106.4</v>
+        <v>106.89</v>
       </c>
       <c r="E13">
         <v>80.59</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1329,16 +1520,16 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <v>209</v>
+        <v>240</v>
       </c>
       <c r="D14">
-        <v>111.57</v>
+        <v>112.06</v>
       </c>
       <c r="E14">
         <v>80.75</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1346,16 +1537,16 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="D15">
-        <v>111.11</v>
+        <v>110.3</v>
       </c>
       <c r="E15">
         <v>80.91</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1363,16 +1554,16 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D16">
-        <v>107.14</v>
+        <v>107</v>
       </c>
       <c r="E16">
-        <v>81.07</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>81.069999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1383,13 +1574,13 @@
         <v>60</v>
       </c>
       <c r="D17">
-        <v>49.58</v>
+        <v>49.79</v>
       </c>
       <c r="E17">
         <v>81.23</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1397,16 +1588,16 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18">
-        <v>38.89</v>
+        <v>38.81</v>
       </c>
       <c r="E18">
-        <v>81.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1414,16 +1605,16 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="D19">
-        <v>104.49</v>
+        <v>104.35</v>
       </c>
       <c r="E19">
         <v>81.56</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1431,16 +1622,16 @@
         <v>30</v>
       </c>
       <c r="C20">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D20">
-        <v>108.77</v>
+        <v>108.89</v>
       </c>
       <c r="E20">
         <v>81.72</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1448,16 +1639,16 @@
         <v>31</v>
       </c>
       <c r="C21">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D21">
-        <v>113.45</v>
+        <v>114.05</v>
       </c>
       <c r="E21">
         <v>81.88</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1465,16 +1656,16 @@
         <v>32</v>
       </c>
       <c r="C22">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="D22">
-        <v>112.36</v>
+        <v>111.76</v>
       </c>
       <c r="E22">
         <v>82.04</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1482,13 +1673,132 @@
         <v>33</v>
       </c>
       <c r="C23">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="D23">
-        <v>110.4</v>
+        <v>109.94</v>
       </c>
       <c r="E23">
         <v>82.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>107</v>
+      </c>
+      <c r="D24">
+        <v>50.87</v>
+      </c>
+      <c r="E24">
+        <v>82.36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>67</v>
+      </c>
+      <c r="D25">
+        <v>39.33</v>
+      </c>
+      <c r="E25">
+        <v>82.53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26">
+        <v>223</v>
+      </c>
+      <c r="D26">
+        <v>106.72</v>
+      </c>
+      <c r="E26">
+        <v>82.69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>189</v>
+      </c>
+      <c r="D27">
+        <v>110.3</v>
+      </c>
+      <c r="E27">
+        <v>82.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>178</v>
+      </c>
+      <c r="D28">
+        <v>115.2</v>
+      </c>
+      <c r="E28">
+        <v>83.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29">
+        <v>199</v>
+      </c>
+      <c r="D29">
+        <v>113.32</v>
+      </c>
+      <c r="E29">
+        <v>83.17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30">
+        <v>266</v>
+      </c>
+      <c r="D30">
+        <v>112.89</v>
+      </c>
+      <c r="E30">
+        <v>83.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>